<commit_message>
Integracion de la informacion scriots con parches difusos
</commit_message>
<xml_diff>
--- a/Experimentos/Exp de Gabor/Integracion de la informacion/ParametrosAyB.xlsx
+++ b/Experimentos/Exp de Gabor/Integracion de la informacion/ParametrosAyB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UdeSA\Desktop\Antonella\Doctorado (1)\Exp de Gabor\Exp de Gabor\Integracion de la informacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antonella\Experimentos\Exp de Gabor\Integracion de la informacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -125,6 +125,1757 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Hoja1!$B:$B</c:f>
+              <c:strCache>
+                <c:ptCount val="152"/>
+                <c:pt idx="0">
+                  <c:v>FrecuenciaEspacial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0,028117897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0,028454898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0,028515114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0,033856245</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0,03392957</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0,02893065</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0,033701855</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0,028507351</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0,02846187</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0,034110893</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0,034309666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0,028626531</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0,028247894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0,034374564</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0,033725308</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0,028397601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0,028595725</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0,033982605</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0,028330158</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0,02857275</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0,033989041</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0,033652771</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0,034171566</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0,028355413</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0,033771689</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0,033755814</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0,028219571</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0,03376132</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0,033499891</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0,033856207</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0,028354717</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0,028547173</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0,028758251</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0,028439366</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0,028537459</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0,028436629</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0,034088036</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0,028393891</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0,03364352</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0,033879699</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0,028693036</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0,033483635</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0,033715657</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0,034078049</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0,034023754</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0,028772482</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0,028471387</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0,033782492</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0,028711731</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0,028556484</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0,028342726</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0,033889766</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0,033959999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0,033665188</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0,03345197</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0,028575874</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0,033987067</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0,03411718</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0,028531086</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0,033648447</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0,028500991</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0,034009852</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0,033751335</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0,028289019</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0,028903835</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0,028657457</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0,03402206</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0,028409993</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0,02835559</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0,028869739</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0,028250049</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0,028611411</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0,033904901</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0,034141241</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0,034059218</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0,028779566</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0,033825118</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0,033804854</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0,034121593</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0,028335699</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0,033821525</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0,034120699</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0,028545272</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0,033905838</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0,028506646</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0,034002371</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0,028573981</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0,03371454</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0,033760672</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0,03397231</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0,033968515</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0,033946786</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0,034254277</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0,028311273</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0,033725892</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0,034255046</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0,02807997</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0,028163618</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0,028459683</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0,028237465</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0,034077847</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0,033830925</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0,034041022</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0,03390248</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0,028339781</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0,028165561</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0,033861046</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0,033909113</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0,033738382</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0,034226205</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0,033900813</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0,028248367</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0,028338738</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0,034062426</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0,033670029</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0,028325674</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0,028515574</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0,028347199</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0,034050491</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0,034046824</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0,028405375</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0,028570435</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0,028098317</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0,034414698</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0,028477316</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0,028475499</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0,034177103</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0,033620777</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0,03392057</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0,033890922</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0,028209913</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0,028827188</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0,033759535</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0,033860353</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0,034047025</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0,034029</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0,03386086</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0,034073121</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0,028719352</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0,028808836</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0,028467103</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0,028224554</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0,028349335</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0,028653582</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0,033658083</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0,028000044</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0,028620289</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0,02844391</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0,034305437</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0,028624951</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0,033649556</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D:$D</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.369866345245597</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.071037233132188</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.9982272857429</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.2038916028961</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.968145820598593</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.890648429862409</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.524612461558299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96.508668593333496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.500679714211799</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.215833466435498</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.150615169344405</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>97.247230545717301</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94.340236614351795</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>63.519077430824701</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59.628154069129799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95.494243127605003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.06851619359999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61.119735380497495</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95.807683538860502</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>97.434921498953003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>61.368722834518593</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>58.974062204895297</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>62.073501619574898</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>95.289589788199606</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>59.795980634423493</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>59.723953065391996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>94.651711497527998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59.213835858431999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>58.648227516815297</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>60.382619638082801</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>95.379885725974702</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>96.492689296522698</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>98.173147379378804</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>96.074114956131595</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>96.904221614918001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.924558333574097</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>61.404438209377197</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95.595977763110199</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>59.373281646197498</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60.452992053030599</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>98.041540050284198</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>57.806333718549993</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>59.671506106946801</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>61.808557062204507</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>61.694022790144096</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>98.177472018280497</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96.175376013923994</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>60.0588480780035</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>97.682029398563799</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>96.699293062064001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>95.334035939912596</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>60.968726170368505</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>61.310406174039798</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>58.678094566176796</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>58.079882398284397</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>96.504680725292104</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>61.353886701851799</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>62.045457311574104</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>96.5766868246602</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>58.900115234205799</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>96.674313870867806</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>61.093038251227206</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>59.823626974468901</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>95.125475766462202</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>98.865472238962099</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>97.658549220859001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>61.499169023446797</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>96.400449198418102</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>95.424497817097503</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>98.821593323841398</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>95.340844677694406</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96.6496667171957</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>61.038457968098903</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>62.251396863175103</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>61.6539616399956</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>98.388163021703107</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>59.981787707105404</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>59.906635596905303</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>61.843282243956402</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>95.416169136543303</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>60.337055243167505</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>61.896775010215997</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>96.780894998191599</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>60.857887993689296</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>96.305479356857603</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>61.085281333288201</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>96.809120190822597</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>59.651531533259707</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>59.780109094705502</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>60.770254281772992</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>61.050527999669704</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>61.345719824181302</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>62.909030759480402</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94.9507888035088</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>59.134201286126</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>62.821445237007502</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>93.504363063965002</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>94.141728071069892</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>96.348109660715792</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>95.176118593094202</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>61.895076489497001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>60.112656732339396</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>61.202351859733497</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>60.523484304418993</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>95.711214414252396</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>94.423966179962406</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>60.647537722086696</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>60.524966343389096</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>59.649218570689797</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>62.606997235370599</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>60.8232589551179</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>94.8101423915694</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>95.261025753119398</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>61.766429036685501</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>59.219024555946397</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>94.893201561226604</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>96.283026624412599</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>95.097096446677298</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>61.857674849880993</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>61.526736455963807</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>95.763152041792495</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>96.896212994170298</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>93.801105173591807</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>63.560409889554201</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>96.502067266261903</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>96.144086986158712</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>62.319561820170996</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>59.169120729825998</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>60.527632698776003</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>60.640102934239202</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>94.604995076871106</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>98.458826231353299</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>59.527199295490298</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>60.472795423691196</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>61.273211643981796</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>61.524911204989195</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>60.238087632269398</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>61.571081157574405</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>98.34702907635851</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>98.296872667802504</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>96.573683792902798</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>94.888076767077607</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>95.4293449490428</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>97.392662352481594</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>59.199143296204305</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>93.4186576132482</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>96.856409971149205</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>95.879520219208501</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>63.237568372850603</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>97.193716252801295</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>59.291900536986397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D331-4E42-B7F1-B579EC6C79C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2062352400"/>
+        <c:axId val="2062352816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2062352400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062352816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2062352816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062352400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,7 +2145,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -405,10 +2156,10 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +2179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5.6235794479149801</v>
       </c>
@@ -449,8 +2200,12 @@
         <f>IF(C2="Left","left","right")</f>
         <v>left</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>MIN(A2:A152)</f>
+        <v>5.60000875324811</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.6909795737274704</v>
       </c>
@@ -471,8 +2226,12 @@
         <f t="shared" ref="F3:F66" si="1">IF(C3="Left","left","right")</f>
         <v>left</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="e">
+        <f>Min.Si.Con</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.7030227731469596</v>
       </c>
@@ -494,7 +2253,7 @@
         <v>left</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.7712490071333997</v>
       </c>
@@ -516,7 +2275,7 @@
         <v>right</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6.7859139669426396</v>
       </c>
@@ -538,7 +2297,7 @@
         <v>right</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.7861300224522001</v>
       </c>
@@ -560,7 +2319,7 @@
         <v>left</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.7403710947164202</v>
       </c>
@@ -582,7 +2341,7 @@
         <v>right</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.7014702969031301</v>
       </c>
@@ -604,7 +2363,7 @@
         <v>left</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.6923740224344801</v>
       </c>
@@ -626,7 +2385,7 @@
         <v>left</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6.8221786052128097</v>
       </c>
@@ -648,7 +2407,7 @@
         <v>right</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6.8619331480848498</v>
       </c>
@@ -670,7 +2429,7 @@
         <v>right</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5.7253062532267798</v>
       </c>
@@ -692,7 +2451,7 @@
         <v>left</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5.6495788253212202</v>
       </c>
@@ -714,7 +2473,7 @@
         <v>left</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6.8749127966295003</v>
       </c>
@@ -736,7 +2495,7 @@
         <v>right</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6.7450616494521398</v>
       </c>
@@ -2545,7 +4304,7 @@
         <v>5.6159940173659697</v>
       </c>
       <c r="B98">
-        <f t="shared" ref="B98:B129" si="5">A98/200</f>
+        <f t="shared" ref="B98:B120" si="5">A98/200</f>
         <v>2.8079970086829848E-2</v>
       </c>
       <c r="C98" t="s">
@@ -3753,5 +5512,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>